<commit_message>
Planilha de requisitos atualizada
Planilha de requisitos atualizada
</commit_message>
<xml_diff>
--- a/Docs/Planilha_requisitos.xlsx
+++ b/Docs/Planilha_requisitos.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\GitHub\Projeto-inovacao\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>RF01</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Banco de dados para plantas</t>
   </si>
   <si>
-    <t>O usuário pode selecionar a planta desejada</t>
-  </si>
-  <si>
     <t>Sensores conversarem com o arduíno</t>
   </si>
   <si>
@@ -158,22 +155,55 @@
     <t>Ter conexão com a internet</t>
   </si>
   <si>
-    <t>Tela de cadastro para o usuário</t>
-  </si>
-  <si>
-    <t>Tela  de login para o usuário</t>
-  </si>
-  <si>
-    <t>Usuário ter acesso aos dados no Arduíno</t>
-  </si>
-  <si>
     <t>Banco de dados conectado à nuvem</t>
+  </si>
+  <si>
+    <t>Protótipo possuir nome da empresa/grupo e a nossa proposta</t>
+  </si>
+  <si>
+    <t>Protótipo explicar o nosso projeto principal</t>
+  </si>
+  <si>
+    <t>Protótipo possuir uma área "sobre nós"</t>
+  </si>
+  <si>
+    <t>Protótipo possuir uma área "curiosidades sobre o mundo orgânico"</t>
+  </si>
+  <si>
+    <t>Protótipo possuir uma área "e-commerce"</t>
+  </si>
+  <si>
+    <t>Botão que direciona à homepage do protótipo</t>
+  </si>
+  <si>
+    <t>Protótipo mostrar o simulador financeiro</t>
+  </si>
+  <si>
+    <t>Protótipo com tela de cadastro para o usuário</t>
+  </si>
+  <si>
+    <t>Protótipo com tela  de login para o usuário</t>
+  </si>
+  <si>
+    <t>Usuário ter acesso aos gráficos forncecidos pelo Arduíno através do protótipo</t>
+  </si>
+  <si>
+    <t>O usuário pode ver dados do banco de dados das plantas através do protótipo</t>
+  </si>
+  <si>
+    <t>Protótipo possuir a Logo da equipe em todas as telas</t>
+  </si>
+  <si>
+    <t>Arduíno conseguir controlar a estufa</t>
+  </si>
+  <si>
+    <t>Site completo no futuro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,12 +520,12 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="1.85546875" customWidth="1"/>
@@ -533,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -558,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -568,7 +598,7 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
         <v>36</v>
@@ -583,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -593,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -604,8 +634,8 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>46</v>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -615,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
@@ -626,13 +656,18 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
         <v>35</v>
@@ -643,12 +678,18 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="F7" t="s">
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
         <v>35</v>
@@ -659,6 +700,12 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="F8" t="s">
         <v>22</v>
@@ -669,6 +716,12 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="F9" t="s">
         <v>23</v>
@@ -679,6 +732,12 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="F10" t="s">
         <v>24</v>
@@ -689,6 +748,12 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="F11" t="s">
         <v>25</v>
@@ -699,6 +764,12 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="F12" t="s">
         <v>26</v>
@@ -709,6 +780,12 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="F13" t="s">
         <v>27</v>
@@ -719,6 +796,12 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="F14" t="s">
         <v>28</v>
@@ -728,6 +811,12 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" t="s">

</xml_diff>

<commit_message>
Planilha de requisitos - necessita revisão
Necessita revisão
</commit_message>
<xml_diff>
--- a/Docs/Planilha_requisitos.xlsx
+++ b/Docs/Planilha_requisitos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>RF01</t>
   </si>
@@ -68,12 +68,6 @@
     <t>RF14</t>
   </si>
   <si>
-    <t>RF15</t>
-  </si>
-  <si>
-    <t>RF16</t>
-  </si>
-  <si>
     <t>RNF01</t>
   </si>
   <si>
@@ -90,36 +84,6 @@
   </si>
   <si>
     <t>RNF06</t>
-  </si>
-  <si>
-    <t>RNF07</t>
-  </si>
-  <si>
-    <t>RNF08</t>
-  </si>
-  <si>
-    <t>RNF09</t>
-  </si>
-  <si>
-    <t>RNF10</t>
-  </si>
-  <si>
-    <t>RNF11</t>
-  </si>
-  <si>
-    <t>RNF12</t>
-  </si>
-  <si>
-    <t>RNF13</t>
-  </si>
-  <si>
-    <t>RNF14</t>
-  </si>
-  <si>
-    <t>RNF15</t>
-  </si>
-  <si>
-    <t>RNF16</t>
   </si>
   <si>
     <t>Descrição</t>
@@ -221,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -229,14 +193,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +509,7 @@
     <col min="2" max="2" width="69.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
@@ -536,312 +517,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43584</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3">
+        <v>43584</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43584</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3">
+        <v>43584</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43542</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43542</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="3">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43542</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="3">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3">
+        <v>43542</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3">
+        <v>43542</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3">
+        <v>43542</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43619</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43542</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43542</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43584</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43619</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="F13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="F15" t="s">
-        <v>29</v>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3">
+        <v>43619</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="1"/>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
       <c r="I17" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planilha de Requisitos - Finalizada
Os requisitos funcionais e não funcionais estão finalizados, se quiserem incluir ou modificar alguma coisa, fiquem à vontade.
</commit_message>
<xml_diff>
--- a/Docs/Planilha_requisitos.xlsx
+++ b/Docs/Planilha_requisitos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Projeto-inovacao\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\GitHub\Projeto-inovacao\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958ACEED-78C5-4200-B8BB-81AC795C4486}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>RF01</t>
   </si>
@@ -177,40 +176,22 @@
     <t>RNF10</t>
   </si>
   <si>
-    <t>RNF11</t>
-  </si>
-  <si>
-    <t>RNF12</t>
-  </si>
-  <si>
-    <t>RNF13</t>
-  </si>
-  <si>
-    <t>RNF14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">banco de dados de temperatura </t>
-  </si>
-  <si>
-    <t>banco de dados usário</t>
-  </si>
-  <si>
     <t>sistema fazer backup periodicamente</t>
   </si>
   <si>
     <t>guardar backup em um local seguro</t>
   </si>
   <si>
-    <t>verificar se a bugs periodiacamente</t>
-  </si>
-  <si>
-    <t>verificar se a feedback ou sugestões dos usuários</t>
+    <t xml:space="preserve">banco de dados para temperatura </t>
+  </si>
+  <si>
+    <t>banco de dados para usuário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,11 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,16 +522,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="69.85546875" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
@@ -588,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="3">
-        <v>43584</v>
+        <v>43542</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>
@@ -603,10 +586,10 @@
         <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3">
-        <v>43584</v>
+        <v>43542</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
@@ -617,13 +600,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3">
-        <v>43584</v>
+        <v>43542</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -635,7 +618,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="3">
-        <v>43584</v>
+        <v>43542</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -646,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <v>43542</v>
@@ -658,10 +641,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="3">
         <v>43542</v>
@@ -672,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -684,10 +667,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" s="3">
         <v>43542</v>
@@ -698,10 +681,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>43542</v>
@@ -724,10 +707,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <v>43542</v>
@@ -750,10 +733,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>43542</v>
@@ -762,22 +745,24 @@
         <v>46</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="I8" s="3">
+        <v>43542</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3">
         <v>43542</v>
@@ -786,130 +771,120 @@
         <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="I9" s="3">
+        <v>43542</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3">
-        <v>43619</v>
+        <v>43584</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3">
+        <v>43619</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3">
-        <v>43542</v>
+        <v>43584</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3">
+        <v>43619</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3">
-        <v>43542</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="3"/>
+        <v>43584</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3">
-        <v>43584</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="3"/>
+        <v>43619</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3">
         <v>43619</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -924,26 +899,23 @@
       <c r="D15" s="3">
         <v>43619</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C17 C1:C2 H1:H18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14:H18 H1:H11 C1 C3:C11 C13 C14:C15">
       <formula1>$L$1:$L$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Planilha de Requisitos Finalizada e Formatarda
Agora sim está certa, sintam-se à vontade de fazer qualquer alteração e inclusão, atenção aos erros ortográficos.
</commit_message>
<xml_diff>
--- a/Docs/Planilha_requisitos.xlsx
+++ b/Docs/Planilha_requisitos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>RF01</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Protótipo possuir uma área "e-commerce"</t>
   </si>
   <si>
-    <t>Botão que direciona à homepage do protótipo</t>
-  </si>
-  <si>
     <t>Protótipo mostrar o simulador financeiro</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Protótipo possuir a Logo da equipe em todas as telas</t>
   </si>
   <si>
-    <t>Arduíno conseguir controlar a estufa</t>
-  </si>
-  <si>
     <t>Site completo no futuro</t>
   </si>
   <si>
@@ -173,19 +167,19 @@
     <t>RNF09</t>
   </si>
   <si>
-    <t>RNF10</t>
-  </si>
-  <si>
-    <t>sistema fazer backup periodicamente</t>
-  </si>
-  <si>
-    <t>guardar backup em um local seguro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">banco de dados para temperatura </t>
-  </si>
-  <si>
-    <t>banco de dados para usuário</t>
+    <t xml:space="preserve">Banco de dados para temperatura </t>
+  </si>
+  <si>
+    <t>Banco de dados para usuário</t>
+  </si>
+  <si>
+    <t>Sistema fazer backup periodicamente</t>
+  </si>
+  <si>
+    <t>Arduíno ter o controle da estufa</t>
+  </si>
+  <si>
+    <t>Protótipo possuir um botão que direciona à homepage</t>
   </si>
 </sst>
 </file>
@@ -526,18 +520,20 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="73.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="48.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -571,10 +567,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3">
         <v>43542</v>
@@ -583,10 +579,10 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3">
         <v>43542</v>
@@ -600,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>23</v>
@@ -612,10 +608,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="3">
         <v>43542</v>
@@ -629,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -641,10 +637,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3">
         <v>43542</v>
@@ -655,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -667,10 +663,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3">
         <v>43542</v>
@@ -681,10 +677,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>43542</v>
@@ -693,10 +689,10 @@
         <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3">
         <v>43542</v>
@@ -707,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
@@ -719,10 +715,10 @@
         <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" s="3">
         <v>43542</v>
@@ -733,22 +729,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3">
         <v>43542</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="3">
         <v>43542</v>
@@ -759,22 +755,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3">
         <v>43542</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" s="3">
         <v>43542</v>
@@ -785,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -794,10 +790,10 @@
         <v>43584</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -819,25 +815,17 @@
       <c r="D11" s="3">
         <v>43584</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="3">
-        <v>43619</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
@@ -846,16 +834,13 @@
         <v>43584</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>23</v>
@@ -864,9 +849,6 @@
         <v>43619</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -882,16 +864,13 @@
         <v>43619</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -900,9 +879,6 @@
         <v>43619</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="1"/>
@@ -915,7 +891,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14:H18 H1:H11 C1 C3:C11 C13 C14:C15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C8 H1:H11 H16:H18 C10 C12:C15">
       <formula1>$L$1:$L$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Atualizado os arquivos de Docs (Check-in e Backup)
</commit_message>
<xml_diff>
--- a/Docs/Planilha_requisitos.xlsx
+++ b/Docs/Planilha_requisitos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cleitom\Desktop\Projeto-inovacao\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\GitHub\Projeto-inovacao\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C69219-8CA3-4AEE-8E9A-C24517C99785}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>RF01</t>
   </si>
@@ -153,6 +152,9 @@
     <t>O usuário pode ver dados do banco de dados das plantas através do protótipo</t>
   </si>
   <si>
+    <t>Protótipo possuir a Logo da equipe em todas as telas</t>
+  </si>
+  <si>
     <t>Site completo no futuro</t>
   </si>
   <si>
@@ -178,18 +180,12 @@
   </si>
   <si>
     <t>Protótipo possuir um botão que direciona à homepage</t>
-  </si>
-  <si>
-    <t>Protótipo possuir a Logo da equipe na home page</t>
-  </si>
-  <si>
-    <t>desejável</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,11 +230,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,11 +516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
@@ -598,10 +596,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3">
         <v>43542</v>
@@ -627,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -653,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -679,10 +677,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <v>43542</v>
@@ -705,10 +703,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <v>43542</v>
@@ -731,19 +729,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3">
         <v>43542</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>24</v>
@@ -757,19 +755,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3">
         <v>43542</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>24</v>
@@ -792,10 +790,10 @@
         <v>43584</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -817,7 +815,10 @@
       <c r="D11" s="3">
         <v>43584</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -832,13 +833,14 @@
       <c r="D12" s="3">
         <v>43584</v>
       </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>23</v>
@@ -846,6 +848,7 @@
       <c r="D13" s="3">
         <v>43619</v>
       </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -860,13 +863,14 @@
       <c r="D14" s="3">
         <v>43619</v>
       </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -874,20 +878,24 @@
       <c r="D15" s="3">
         <v>43619</v>
       </c>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H11 H16:H18 C10 C12:C15 C9 C1:C2 C3:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C8 H1:H11 H16:H18 C10 C12:C15">
       <formula1>$L$1:$L$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>